<commit_message>
new page with colored backgrounds (intent is to shwo differences when drawing selection rectangle which should be improved)
</commit_message>
<xml_diff>
--- a/meja-samples/testdata/test.xlsx
+++ b/meja-samples/testdata/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Alignment Test" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Border Test" sheetId="3" r:id="rId3"/>
     <sheet name="Font Test" sheetId="4" r:id="rId4"/>
     <sheet name="Palette" sheetId="5" r:id="rId5"/>
+    <sheet name="Background" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1041,7 +1042,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1238,8 +1239,14 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="374">
+  <fills count="384">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3478,8 +3485,68 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -3538,11 +3605,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="453">
+  <cellXfs count="506">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4779,6 +4926,67 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="374" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="375" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="374" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="374" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="374" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="375" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="375" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="375" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="376" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="377" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="376" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="376" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="376" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="377" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="377" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="377" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="376" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="377" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="378" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="379" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="378" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="378" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="379" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="379" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="380" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="381" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="380" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="380" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="380" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="381" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="381" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="381" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="380" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="381" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="382" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="383" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="382" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="382" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="383" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="383" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="382" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="383" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="distributed"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5236,11 +5444,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5389,22 +5597,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8" t="s">
+      <c r="B8" s="501" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="502" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="503" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="504" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="505" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="505" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5526,7 +5734,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5703,7 +5911,7 @@
   <dimension ref="B1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5851,7 +6059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -7920,4 +8128,139 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="453"/>
+      <c r="B1" s="454"/>
+      <c r="C1" s="455"/>
+      <c r="D1" s="453"/>
+      <c r="E1" s="456"/>
+      <c r="F1" s="455"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="457"/>
+      <c r="B2" s="458"/>
+      <c r="C2" s="459"/>
+      <c r="D2" s="460"/>
+      <c r="E2" s="461"/>
+      <c r="F2" s="462"/>
+    </row>
+    <row r="3" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="463"/>
+      <c r="B3" s="458"/>
+      <c r="C3" s="464"/>
+      <c r="D3" s="463"/>
+      <c r="E3" s="461"/>
+      <c r="F3" s="464"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="453"/>
+      <c r="B4" s="465"/>
+      <c r="C4" s="455"/>
+      <c r="D4" s="453"/>
+      <c r="E4" s="466"/>
+      <c r="F4" s="455"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="467"/>
+      <c r="B5" s="468"/>
+      <c r="C5" s="469"/>
+      <c r="D5" s="470"/>
+      <c r="E5" s="471"/>
+      <c r="F5" s="472"/>
+    </row>
+    <row r="6" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="473"/>
+      <c r="B6" s="474"/>
+      <c r="C6" s="475"/>
+      <c r="D6" s="473"/>
+      <c r="E6" s="476"/>
+      <c r="F6" s="475"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="463"/>
+      <c r="B7" s="477"/>
+      <c r="C7" s="464"/>
+      <c r="D7" s="463"/>
+      <c r="E7" s="478"/>
+      <c r="F7" s="464"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="479"/>
+      <c r="B8" s="477"/>
+      <c r="C8" s="480"/>
+      <c r="D8" s="481"/>
+      <c r="E8" s="478"/>
+      <c r="F8" s="482"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="463"/>
+      <c r="B9" s="477"/>
+      <c r="C9" s="464"/>
+      <c r="D9" s="463"/>
+      <c r="E9" s="478"/>
+      <c r="F9" s="464"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="453"/>
+      <c r="B10" s="483"/>
+      <c r="C10" s="455"/>
+      <c r="D10" s="453"/>
+      <c r="E10" s="484"/>
+      <c r="F10" s="455"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="485"/>
+      <c r="B11" s="486"/>
+      <c r="C11" s="487"/>
+      <c r="D11" s="488"/>
+      <c r="E11" s="489"/>
+      <c r="F11" s="490"/>
+    </row>
+    <row r="12" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="473"/>
+      <c r="B12" s="491"/>
+      <c r="C12" s="475"/>
+      <c r="D12" s="473"/>
+      <c r="E12" s="492"/>
+      <c r="F12" s="475"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="463"/>
+      <c r="B13" s="493"/>
+      <c r="C13" s="464"/>
+      <c r="D13" s="463"/>
+      <c r="E13" s="494"/>
+      <c r="F13" s="464"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="495"/>
+      <c r="B14" s="493"/>
+      <c r="C14" s="496"/>
+      <c r="D14" s="497"/>
+      <c r="E14" s="494"/>
+      <c r="F14" s="498"/>
+    </row>
+    <row r="15" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="473"/>
+      <c r="B15" s="499"/>
+      <c r="C15" s="475"/>
+      <c r="D15" s="473"/>
+      <c r="E15" s="500"/>
+      <c r="F15" s="475"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>